<commit_message>
got code doing stuff
</commit_message>
<xml_diff>
--- a/excel/PCLRWords.xlsx
+++ b/excel/PCLRWords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PsychopathyFuzzyThesis\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109BD1BD-3624-4335-8638-462220B2683F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4C49DA-6D01-4BF3-B55C-B1076EF07D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Glib</t>
   </si>
   <si>
-    <t xml:space="preserve">Importance </t>
-  </si>
-  <si>
     <t xml:space="preserve">Grandiosity </t>
   </si>
   <si>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t>Very Emotionally Controlled</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,10 +871,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -894,13 +894,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -909,13 +909,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -924,13 +924,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -939,13 +939,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -954,13 +954,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -969,13 +969,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -984,13 +984,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -999,13 +999,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -1029,13 +1029,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1044,13 +1044,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1074,13 +1074,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1089,13 +1089,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1104,13 +1104,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1119,46 +1119,46 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,7 +1365,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1373,519 +1373,519 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
         <v>139</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>140</v>
       </c>
-      <c r="D5" t="s">
-        <v>141</v>
-      </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>56</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>59</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
         <v>60</v>
       </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>61</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>62</v>
-      </c>
-      <c r="H8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
         <v>72</v>
       </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>73</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>74</v>
-      </c>
-      <c r="H10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
         <v>76</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>77</v>
       </c>
-      <c r="D11" t="s">
-        <v>78</v>
-      </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" t="s">
         <v>142</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>143</v>
-      </c>
-      <c r="H11" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
         <v>79</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>80</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
         <v>81</v>
       </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>82</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>83</v>
-      </c>
-      <c r="H12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
         <v>87</v>
       </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>89</v>
-      </c>
-      <c r="H13" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
         <v>91</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>92</v>
       </c>
-      <c r="D14" t="s">
-        <v>93</v>
-      </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
         <v>73</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>74</v>
-      </c>
-      <c r="H14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
         <v>94</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>95</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
         <v>96</v>
       </c>
-      <c r="E15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>97</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>98</v>
-      </c>
-      <c r="H15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
         <v>100</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>101</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
         <v>102</v>
       </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>103</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>104</v>
-      </c>
-      <c r="H16" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
         <v>106</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>107</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
         <v>108</v>
       </c>
-      <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>109</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>110</v>
-      </c>
-      <c r="H17" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
         <v>112</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>113</v>
       </c>
-      <c r="D18" t="s">
-        <v>114</v>
-      </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G18" t="s">
         <v>145</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>146</v>
-      </c>
-      <c r="H18" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" t="s">
         <v>115</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>116</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
         <v>117</v>
       </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>118</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>119</v>
-      </c>
-      <c r="H19" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
         <v>121</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>122</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
         <v>123</v>
       </c>
-      <c r="E20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>124</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>125</v>
-      </c>
-      <c r="H20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
         <v>127</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>128</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
         <v>129</v>
       </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>130</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>131</v>
-      </c>
-      <c r="H21" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
         <v>133</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>134</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
         <v>135</v>
       </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>136</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>137</v>
-      </c>
-      <c r="H22" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>